<commit_message>
reran chuffed and kissat with 10min time limit
</commit_message>
<xml_diff>
--- a/results/table 1.xlsx
+++ b/results/table 1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ozgurakgun/repos/github/ozgurakgun/magic-hexagon/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ozgurakgun/repos/github/ozgurakgun/magic-hexagon/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADCC2CA6-BB6A-E34A-9016-CA6F45F3B384}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2576811-12BC-014D-BC38-D64F05F373A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="45160" yWindow="9220" windowWidth="22380" windowHeight="28140" activeTab="1" xr2:uid="{81ED7F14-820B-C144-81AC-28F30AD4118D}"/>
   </bookViews>
@@ -212,9 +212,6 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -226,6 +223,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -786,7 +786,7 @@
   <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30:D35"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.33203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -795,29 +795,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-    </row>
-    <row r="2" spans="1:4" s="5" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+    </row>
+    <row r="2" spans="1:4" s="4" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="2">
+      <c r="A3" s="1">
         <v>3</v>
       </c>
       <c r="B3">
@@ -831,7 +831,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="2">
+      <c r="A4" s="1">
         <v>4</v>
       </c>
       <c r="B4">
@@ -845,7 +845,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="2">
+      <c r="A5" s="1">
         <v>5</v>
       </c>
       <c r="B5">
@@ -859,7 +859,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="2">
+      <c r="A6" s="1">
         <v>6</v>
       </c>
       <c r="B6">
@@ -873,7 +873,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="2">
+      <c r="A7" s="1">
         <v>7</v>
       </c>
       <c r="B7">
@@ -887,7 +887,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="2">
+      <c r="A8" s="1">
         <v>8</v>
       </c>
       <c r="B8">
@@ -901,29 +901,29 @@
       </c>
     </row>
     <row r="10" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="1:4" s="5" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+    </row>
+    <row r="11" spans="1:4" s="4" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="2">
+      <c r="A12" s="1">
         <v>3</v>
       </c>
       <c r="B12">
@@ -937,7 +937,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="2">
+      <c r="A13" s="1">
         <v>4</v>
       </c>
       <c r="B13">
@@ -951,7 +951,7 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="2">
+      <c r="A14" s="1">
         <v>5</v>
       </c>
       <c r="B14">
@@ -965,7 +965,7 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="2">
+      <c r="A15" s="1">
         <v>6</v>
       </c>
       <c r="B15">
@@ -979,7 +979,7 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="2">
+      <c r="A16" s="1">
         <v>7</v>
       </c>
       <c r="B16">
@@ -993,7 +993,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="2">
+      <c r="A17" s="1">
         <v>8</v>
       </c>
       <c r="B17">
@@ -1007,29 +1007,29 @@
       </c>
     </row>
     <row r="19" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-    </row>
-    <row r="20" spans="1:4" s="5" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+    </row>
+    <row r="20" spans="1:4" s="4" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="D20" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="2">
+      <c r="A21" s="1">
         <v>3</v>
       </c>
       <c r="B21">
@@ -1043,7 +1043,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="2">
+      <c r="A22" s="1">
         <v>4</v>
       </c>
       <c r="B22">
@@ -1057,7 +1057,7 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="2">
+      <c r="A23" s="1">
         <v>5</v>
       </c>
       <c r="B23">
@@ -1071,7 +1071,7 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="2">
+      <c r="A24" s="1">
         <v>6</v>
       </c>
       <c r="B24">
@@ -1085,7 +1085,7 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="2">
+      <c r="A25" s="1">
         <v>7</v>
       </c>
       <c r="B25">
@@ -1099,7 +1099,7 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="2">
+      <c r="A26" s="1">
         <v>8</v>
       </c>
       <c r="B26">
@@ -1113,29 +1113,29 @@
       </c>
     </row>
     <row r="28" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
+      <c r="A28" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-    </row>
-    <row r="29" spans="1:4" s="5" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+    </row>
+    <row r="29" spans="1:4" s="4" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B29" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="C29" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D29" s="4" t="s">
+      <c r="D29" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="2">
+      <c r="A30" s="1">
         <v>3</v>
       </c>
       <c r="B30">
@@ -1149,7 +1149,7 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="2">
+      <c r="A31" s="1">
         <v>4</v>
       </c>
       <c r="B31">
@@ -1163,7 +1163,7 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="2">
+      <c r="A32" s="1">
         <v>5</v>
       </c>
       <c r="B32">
@@ -1177,7 +1177,7 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" s="2">
+      <c r="A33" s="1">
         <v>6</v>
       </c>
       <c r="B33">
@@ -1191,7 +1191,7 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" s="2">
+      <c r="A34" s="1">
         <v>7</v>
       </c>
       <c r="B34">
@@ -1205,11 +1205,11 @@
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" s="2">
+      <c r="A35" s="1">
         <v>8</v>
       </c>
       <c r="B35">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C35">
         <v>16</v>

</xml_diff>

<commit_message>
add implied versions of the models and restructure the experiment script
</commit_message>
<xml_diff>
--- a/results/table 1.xlsx
+++ b/results/table 1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ozgurakgun/repos/github/ozgurakgun/magic-hexagon/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2576811-12BC-014D-BC38-D64F05F373A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{882FD714-C879-0B49-8F03-4089CC08797E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45160" yWindow="9220" windowWidth="22380" windowHeight="28140" activeTab="1" xr2:uid="{81ED7F14-820B-C144-81AC-28F30AD4118D}"/>
+    <workbookView xWindow="1140" yWindow="500" windowWidth="44740" windowHeight="28140" activeTab="1" xr2:uid="{81ED7F14-820B-C144-81AC-28F30AD4118D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="14">
   <si>
     <t>Order</t>
   </si>
@@ -126,6 +126,12 @@
       <t>10 minutes</t>
     </r>
   </si>
+  <si>
+    <t>Base model</t>
+  </si>
+  <si>
+    <t>With the implied sums_to constraint</t>
+  </si>
 </sst>
 </file>
 
@@ -156,7 +162,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -189,9 +195,38 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
       <top style="medium">
         <color indexed="64"/>
       </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -199,10 +234,61 @@
     </border>
     <border>
       <left/>
-      <right style="medium">
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -210,11 +296,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -226,6 +309,37 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -783,10 +897,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2880405E-5811-F449-AB85-0B9EC024ACDD}">
-  <dimension ref="A1:D35"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.33203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -794,436 +908,764 @@
     <col min="1" max="1" width="5.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-    </row>
-    <row r="2" spans="1:4" s="4" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+    </row>
+    <row r="2" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="4"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+    </row>
+    <row r="3" spans="1:7" s="3" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="12"/>
+      <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
+      <c r="E3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="13">
         <v>3</v>
       </c>
-      <c r="B3">
-        <v>201</v>
-      </c>
-      <c r="C3">
-        <v>201</v>
-      </c>
-      <c r="D3">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
+      <c r="B4">
+        <v>201</v>
+      </c>
+      <c r="C4">
+        <v>201</v>
+      </c>
+      <c r="D4">
+        <v>201</v>
+      </c>
+      <c r="E4" s="6">
+        <v>201</v>
+      </c>
+      <c r="F4">
+        <v>201</v>
+      </c>
+      <c r="G4">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="13">
         <v>4</v>
       </c>
-      <c r="B4">
+      <c r="B5">
         <v>164</v>
       </c>
-      <c r="C4">
+      <c r="C5">
         <v>164</v>
       </c>
-      <c r="D4">
+      <c r="D5">
         <v>198</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
+      <c r="E5" s="6">
+        <v>198</v>
+      </c>
+      <c r="F5">
+        <v>197</v>
+      </c>
+      <c r="G5">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="13">
         <v>5</v>
       </c>
-      <c r="B5">
+      <c r="B6">
         <v>129</v>
       </c>
-      <c r="C5">
+      <c r="C6">
         <v>128</v>
       </c>
-      <c r="D5">
+      <c r="D6">
         <v>195</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
+      <c r="E6" s="6">
+        <v>194</v>
+      </c>
+      <c r="F6">
+        <v>193</v>
+      </c>
+      <c r="G6">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="13">
         <v>6</v>
       </c>
-      <c r="B6">
+      <c r="B7">
         <v>87</v>
       </c>
-      <c r="C6">
+      <c r="C7">
         <v>85</v>
       </c>
-      <c r="D6">
+      <c r="D7">
         <v>150</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="1">
+      <c r="E7" s="6">
+        <v>191</v>
+      </c>
+      <c r="F7">
+        <v>191</v>
+      </c>
+      <c r="G7">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="13">
         <v>7</v>
       </c>
-      <c r="B7">
+      <c r="B8">
         <v>37</v>
       </c>
-      <c r="C7">
+      <c r="C8">
         <v>37</v>
       </c>
-      <c r="D7">
+      <c r="D8">
         <v>73</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="1">
+      <c r="E8" s="6">
+        <v>190</v>
+      </c>
+      <c r="F8">
+        <v>189</v>
+      </c>
+      <c r="G8">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="13">
         <v>8</v>
       </c>
-      <c r="B8">
+      <c r="B9">
         <v>16</v>
       </c>
-      <c r="C8">
+      <c r="C9">
         <v>16</v>
       </c>
-      <c r="D8">
+      <c r="D9">
         <v>20</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+      <c r="E9" s="6">
+        <v>188</v>
+      </c>
+      <c r="F9">
+        <v>188</v>
+      </c>
+      <c r="G9">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-    </row>
-    <row r="11" spans="1:4" s="4" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+    </row>
+    <row r="12" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B12" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="4"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+    </row>
+    <row r="13" spans="1:7" s="3" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="12"/>
+      <c r="B13" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C13" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D13" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="1">
+      <c r="E13" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="13">
         <v>3</v>
       </c>
-      <c r="B12">
-        <v>201</v>
-      </c>
-      <c r="C12">
-        <v>201</v>
-      </c>
-      <c r="D12">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="1">
+      <c r="B14">
+        <v>201</v>
+      </c>
+      <c r="C14">
+        <v>201</v>
+      </c>
+      <c r="D14">
+        <v>201</v>
+      </c>
+      <c r="E14" s="6">
+        <v>201</v>
+      </c>
+      <c r="F14">
+        <v>201</v>
+      </c>
+      <c r="G14">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="13">
         <v>4</v>
       </c>
-      <c r="B13">
+      <c r="B15">
         <v>167</v>
       </c>
-      <c r="C13">
+      <c r="C15">
         <v>167</v>
       </c>
-      <c r="D13">
+      <c r="D15">
         <v>199</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="1">
+      <c r="E15" s="6">
+        <v>199</v>
+      </c>
+      <c r="F15">
+        <v>199</v>
+      </c>
+      <c r="G15">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="13">
         <v>5</v>
       </c>
-      <c r="B14">
+      <c r="B16">
         <v>131</v>
       </c>
-      <c r="C14">
+      <c r="C16">
         <v>131</v>
       </c>
-      <c r="D14">
+      <c r="D16">
         <v>195</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="1">
+      <c r="E16" s="6">
+        <v>194</v>
+      </c>
+      <c r="F16">
+        <v>193</v>
+      </c>
+      <c r="G16">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="13">
         <v>6</v>
       </c>
-      <c r="B15">
+      <c r="B17">
         <v>92</v>
       </c>
-      <c r="C15">
+      <c r="C17">
         <v>87</v>
       </c>
-      <c r="D15">
+      <c r="D17">
         <v>182</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="1">
+      <c r="E17" s="6">
+        <v>191</v>
+      </c>
+      <c r="F17">
+        <v>191</v>
+      </c>
+      <c r="G17">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="13">
         <v>7</v>
       </c>
-      <c r="B16">
+      <c r="B18">
         <v>37</v>
       </c>
-      <c r="C16">
+      <c r="C18">
         <v>37</v>
       </c>
-      <c r="D16">
+      <c r="D18">
         <v>85</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="1">
+      <c r="E18" s="6">
+        <v>190</v>
+      </c>
+      <c r="F18">
+        <v>189</v>
+      </c>
+      <c r="G18">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="13">
         <v>8</v>
       </c>
-      <c r="B17">
+      <c r="B19">
         <v>16</v>
       </c>
-      <c r="C17">
+      <c r="C19">
         <v>16</v>
       </c>
-      <c r="D17">
+      <c r="D19">
         <v>41</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
+      <c r="E19" s="6">
+        <v>188</v>
+      </c>
+      <c r="F19">
+        <v>188</v>
+      </c>
+      <c r="G19">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-    </row>
-    <row r="20" spans="1:4" s="4" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+    </row>
+    <row r="22" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B22" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22" s="4"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+    </row>
+    <row r="23" spans="1:7" s="3" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="12"/>
+      <c r="B23" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C23" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D23" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="1">
+      <c r="E23" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="13">
         <v>3</v>
       </c>
-      <c r="B21">
-        <v>201</v>
-      </c>
-      <c r="C21">
-        <v>201</v>
-      </c>
-      <c r="D21">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="1">
+      <c r="B24">
+        <v>201</v>
+      </c>
+      <c r="C24">
+        <v>201</v>
+      </c>
+      <c r="D24">
+        <v>201</v>
+      </c>
+      <c r="E24" s="6">
+        <v>201</v>
+      </c>
+      <c r="F24">
+        <v>201</v>
+      </c>
+      <c r="G24">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="13">
         <v>4</v>
       </c>
-      <c r="B22">
+      <c r="B25">
         <v>168</v>
       </c>
-      <c r="C22">
+      <c r="C25">
         <v>169</v>
       </c>
-      <c r="D22">
+      <c r="D25">
         <v>199</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="1">
+      <c r="E25" s="6">
+        <v>200</v>
+      </c>
+      <c r="F25">
+        <v>200</v>
+      </c>
+      <c r="G25">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" s="13">
         <v>5</v>
       </c>
-      <c r="B23">
+      <c r="B26">
         <v>134</v>
       </c>
-      <c r="C23">
+      <c r="C26">
         <v>133</v>
       </c>
-      <c r="D23">
+      <c r="D26">
         <v>195</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="1">
+      <c r="E26" s="6">
+        <v>194</v>
+      </c>
+      <c r="F26">
+        <v>196</v>
+      </c>
+      <c r="G26">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" s="13">
         <v>6</v>
       </c>
-      <c r="B24">
+      <c r="B27">
         <v>94</v>
       </c>
-      <c r="C24">
+      <c r="C27">
         <v>90</v>
       </c>
-      <c r="D24">
+      <c r="D27">
         <v>182</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="1">
+      <c r="E27" s="6">
+        <v>192</v>
+      </c>
+      <c r="F27">
+        <v>191</v>
+      </c>
+      <c r="G27">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" s="13">
         <v>7</v>
       </c>
-      <c r="B25">
+      <c r="B28">
         <v>38</v>
       </c>
-      <c r="C25">
+      <c r="C28">
         <v>37</v>
       </c>
-      <c r="D25">
+      <c r="D28">
         <v>85</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="1">
+      <c r="E28" s="6">
+        <v>190</v>
+      </c>
+      <c r="F28">
+        <v>190</v>
+      </c>
+      <c r="G28">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" s="13">
         <v>8</v>
       </c>
-      <c r="B26">
+      <c r="B29">
         <v>21</v>
       </c>
-      <c r="C26">
+      <c r="C29">
         <v>16</v>
       </c>
-      <c r="D26">
+      <c r="D29">
         <v>42</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
+      <c r="E29" s="6">
+        <v>188</v>
+      </c>
+      <c r="F29">
+        <v>188</v>
+      </c>
+      <c r="G29">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B28" s="5"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
-    </row>
-    <row r="29" spans="1:4" s="4" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
+    </row>
+    <row r="32" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B32" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C32" s="4"/>
+      <c r="D32" s="8"/>
+      <c r="E32" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
+    </row>
+    <row r="33" spans="1:7" s="3" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="10"/>
+      <c r="B33" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C33" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D29" s="3" t="s">
+      <c r="D33" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="1">
+      <c r="E33" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34" s="1">
         <v>3</v>
       </c>
-      <c r="B30">
-        <v>201</v>
-      </c>
-      <c r="C30">
-        <v>201</v>
-      </c>
-      <c r="D30">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="1">
+      <c r="B34">
+        <v>201</v>
+      </c>
+      <c r="C34">
+        <v>201</v>
+      </c>
+      <c r="D34">
+        <v>201</v>
+      </c>
+      <c r="E34" s="6">
+        <v>201</v>
+      </c>
+      <c r="F34">
+        <v>201</v>
+      </c>
+      <c r="G34">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35" s="1">
         <v>4</v>
       </c>
-      <c r="B31">
+      <c r="B35">
         <v>169</v>
       </c>
-      <c r="C31">
+      <c r="C35">
         <v>171</v>
       </c>
-      <c r="D31">
+      <c r="D35">
         <v>200</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="1">
+      <c r="E35" s="6">
+        <v>200</v>
+      </c>
+      <c r="F35">
+        <v>200</v>
+      </c>
+      <c r="G35">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36" s="1">
         <v>5</v>
       </c>
-      <c r="B32">
+      <c r="B36">
         <v>134</v>
       </c>
-      <c r="C32">
+      <c r="C36">
         <v>134</v>
       </c>
-      <c r="D32">
+      <c r="D36">
         <v>196</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" s="1">
+      <c r="E36" s="6">
+        <v>194</v>
+      </c>
+      <c r="F36">
+        <v>196</v>
+      </c>
+      <c r="G36">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37" s="1">
         <v>6</v>
       </c>
-      <c r="B33">
+      <c r="B37">
         <v>94</v>
       </c>
-      <c r="C33">
+      <c r="C37">
         <v>92</v>
       </c>
-      <c r="D33">
+      <c r="D37">
         <v>182</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" s="1">
+      <c r="E37" s="6">
+        <v>192</v>
+      </c>
+      <c r="F37">
+        <v>191</v>
+      </c>
+      <c r="G37">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A38" s="1">
         <v>7</v>
       </c>
-      <c r="B34">
+      <c r="B38">
         <v>40</v>
       </c>
-      <c r="C34">
+      <c r="C38">
         <v>38</v>
       </c>
-      <c r="D34">
+      <c r="D38">
         <v>85</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" s="1">
+      <c r="E38" s="6">
+        <v>190</v>
+      </c>
+      <c r="F38">
+        <v>190</v>
+      </c>
+      <c r="G38">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39" s="1">
         <v>8</v>
       </c>
-      <c r="B35">
+      <c r="B39">
         <v>23</v>
       </c>
-      <c r="C35">
+      <c r="C39">
         <v>16</v>
       </c>
-      <c r="D35">
+      <c r="D39">
         <v>42</v>
       </c>
+      <c r="E39" s="6">
+        <v>188</v>
+      </c>
+      <c r="F39">
+        <v>188</v>
+      </c>
+      <c r="G39">
+        <v>190</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="A28:D28"/>
+  <mergeCells count="16">
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="E22:G22"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="E32:G32"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A11:G11"/>
+    <mergeCell ref="A21:G21"/>
+    <mergeCell ref="A31:G31"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A22:A23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated spreadsheet after a full rerun
</commit_message>
<xml_diff>
--- a/results/table 1.xlsx
+++ b/results/table 1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ozgurakgun/repos/github/ozgurakgun/magic-hexagon/results/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ozgurakgun/repos/github/stacs-cp/magic-hexagon/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCB604B2-B760-D748-B9FB-53114CD599E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1325E6FD-AFFF-A140-8106-37B4A47CA9BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23500" yWindow="500" windowWidth="22380" windowHeight="28140" activeTab="1" xr2:uid="{81ED7F14-820B-C144-81AC-28F30AD4118D}"/>
+    <workbookView xWindow="39040" yWindow="2720" windowWidth="22380" windowHeight="28140" activeTab="1" xr2:uid="{81ED7F14-820B-C144-81AC-28F30AD4118D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -107,8 +107,14 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>5 minutes</t>
+      <t>10 minutes</t>
     </r>
+  </si>
+  <si>
+    <t>Base model</t>
+  </si>
+  <si>
+    <t>With the implied sums_to constraint</t>
   </si>
   <si>
     <r>
@@ -123,14 +129,8 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>10 minutes</t>
+      <t>1 hour</t>
     </r>
-  </si>
-  <si>
-    <t>Base model</t>
-  </si>
-  <si>
-    <t>With the implied sums_to constraint</t>
   </si>
 </sst>
 </file>
@@ -162,7 +162,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -188,15 +188,6 @@
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -274,15 +265,6 @@
     </border>
     <border>
       <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -296,49 +278,40 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -900,7 +873,7 @@
   <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.33203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -909,54 +882,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
     </row>
     <row r="2" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="7"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-    </row>
-    <row r="3" spans="1:7" s="3" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="14"/>
-      <c r="B3" s="2" t="s">
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+    </row>
+    <row r="3" spans="1:7" s="2" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="11"/>
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="6">
+      <c r="A4" s="5">
         <v>3</v>
       </c>
       <c r="B4">
@@ -968,7 +941,7 @@
       <c r="D4">
         <v>201</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="4">
         <v>201</v>
       </c>
       <c r="F4">
@@ -979,20 +952,20 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="6">
+      <c r="A5" s="5">
         <v>4</v>
       </c>
       <c r="B5">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C5">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D5">
         <v>198</v>
       </c>
-      <c r="E5" s="5">
-        <v>198</v>
+      <c r="E5" s="4">
+        <v>199</v>
       </c>
       <c r="F5">
         <v>197</v>
@@ -1002,53 +975,53 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="6">
+      <c r="A6" s="5">
         <v>5</v>
       </c>
       <c r="B6">
         <v>129</v>
       </c>
       <c r="C6">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="D6">
-        <v>199</v>
-      </c>
-      <c r="E6" s="5">
+        <v>195</v>
+      </c>
+      <c r="E6" s="4">
         <v>194</v>
       </c>
       <c r="F6">
         <v>193</v>
       </c>
       <c r="G6">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="6">
+      <c r="A7" s="5">
         <v>6</v>
       </c>
       <c r="B7">
         <v>87</v>
       </c>
       <c r="C7">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D7">
-        <v>169</v>
-      </c>
-      <c r="E7" s="5">
+        <v>181</v>
+      </c>
+      <c r="E7" s="4">
         <v>191</v>
       </c>
       <c r="F7">
         <v>191</v>
       </c>
       <c r="G7">
-        <v>200</v>
+        <v>194</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="6">
+      <c r="A8" s="5">
         <v>7</v>
       </c>
       <c r="B8">
@@ -1058,20 +1031,20 @@
         <v>37</v>
       </c>
       <c r="D8">
-        <v>189</v>
-      </c>
-      <c r="E8" s="5">
+        <v>80</v>
+      </c>
+      <c r="E8" s="4">
         <v>190</v>
       </c>
       <c r="F8">
         <v>189</v>
       </c>
       <c r="G8">
-        <v>200</v>
+        <v>191</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="6">
+      <c r="A9" s="5">
         <v>8</v>
       </c>
       <c r="B9">
@@ -1081,67 +1054,67 @@
         <v>16</v>
       </c>
       <c r="D9">
-        <v>178</v>
-      </c>
-      <c r="E9" s="5">
+        <v>38</v>
+      </c>
+      <c r="E9" s="4">
         <v>188</v>
       </c>
       <c r="F9">
         <v>188</v>
       </c>
       <c r="G9">
-        <v>199</v>
+        <v>190</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
     </row>
     <row r="12" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="15" t="s">
+      <c r="A12" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="7"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="9"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-    </row>
-    <row r="13" spans="1:7" s="3" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="14"/>
-      <c r="B13" s="2" t="s">
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+    </row>
+    <row r="13" spans="1:7" s="2" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="11"/>
+      <c r="B13" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E13" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="F13" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="G13" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="6">
+      <c r="A14" s="5">
         <v>3</v>
       </c>
       <c r="B14">
@@ -1153,7 +1126,7 @@
       <c r="D14">
         <v>201</v>
       </c>
-      <c r="E14" s="5">
+      <c r="E14" s="4">
         <v>201</v>
       </c>
       <c r="F14">
@@ -1164,19 +1137,19 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="6">
+      <c r="A15" s="5">
         <v>4</v>
       </c>
       <c r="B15">
         <v>167</v>
       </c>
       <c r="C15">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="D15">
         <v>199</v>
       </c>
-      <c r="E15" s="5">
+      <c r="E15" s="4">
         <v>199</v>
       </c>
       <c r="F15">
@@ -1187,53 +1160,53 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="6">
+      <c r="A16" s="5">
         <v>5</v>
       </c>
       <c r="B16">
         <v>131</v>
       </c>
       <c r="C16">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D16">
-        <v>199</v>
-      </c>
-      <c r="E16" s="5">
+        <v>195</v>
+      </c>
+      <c r="E16" s="4">
         <v>194</v>
       </c>
       <c r="F16">
         <v>193</v>
       </c>
       <c r="G16">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="6">
+      <c r="A17" s="5">
         <v>6</v>
       </c>
       <c r="B17">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C17">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D17">
-        <v>201</v>
-      </c>
-      <c r="E17" s="5">
+        <v>182</v>
+      </c>
+      <c r="E17" s="4">
         <v>191</v>
       </c>
       <c r="F17">
         <v>191</v>
       </c>
       <c r="G17">
-        <v>200</v>
+        <v>194</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="6">
+      <c r="A18" s="5">
         <v>7</v>
       </c>
       <c r="B18">
@@ -1243,20 +1216,20 @@
         <v>37</v>
       </c>
       <c r="D18">
-        <v>201</v>
-      </c>
-      <c r="E18" s="5">
+        <v>87</v>
+      </c>
+      <c r="E18" s="4">
         <v>190</v>
       </c>
       <c r="F18">
         <v>189</v>
       </c>
       <c r="G18">
-        <v>200</v>
+        <v>192</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="6">
+      <c r="A19" s="5">
         <v>8</v>
       </c>
       <c r="B19">
@@ -1266,67 +1239,67 @@
         <v>16</v>
       </c>
       <c r="D19">
-        <v>199</v>
-      </c>
-      <c r="E19" s="5">
+        <v>41</v>
+      </c>
+      <c r="E19" s="4">
         <v>188</v>
       </c>
       <c r="F19">
         <v>188</v>
       </c>
       <c r="G19">
-        <v>201</v>
+        <v>190</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="9" t="s">
+      <c r="A21" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B21" s="9"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
     </row>
     <row r="22" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="15" t="s">
+      <c r="A22" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B22" s="9" t="s">
+      <c r="B22" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" s="7"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C22" s="9"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9"/>
-    </row>
-    <row r="23" spans="1:7" s="3" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="14"/>
-      <c r="B23" s="2" t="s">
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+    </row>
+    <row r="23" spans="1:7" s="2" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="11"/>
+      <c r="B23" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C23" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D23" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E23" s="4" t="s">
+      <c r="E23" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F23" s="2" t="s">
+      <c r="F23" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G23" s="2" t="s">
+      <c r="G23" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" s="6">
+      <c r="A24" s="5">
         <v>3</v>
       </c>
       <c r="B24">
@@ -1338,7 +1311,7 @@
       <c r="D24">
         <v>201</v>
       </c>
-      <c r="E24" s="5">
+      <c r="E24" s="4">
         <v>201</v>
       </c>
       <c r="F24">
@@ -1349,19 +1322,19 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" s="6">
+      <c r="A25" s="5">
         <v>4</v>
       </c>
       <c r="B25">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C25">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="D25">
-        <v>199</v>
-      </c>
-      <c r="E25" s="5">
+        <v>201</v>
+      </c>
+      <c r="E25" s="4">
         <v>200</v>
       </c>
       <c r="F25">
@@ -1372,19 +1345,19 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A26" s="6">
+      <c r="A26" s="5">
         <v>5</v>
       </c>
       <c r="B26">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C26">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="D26">
-        <v>199</v>
-      </c>
-      <c r="E26" s="5">
+        <v>197</v>
+      </c>
+      <c r="E26" s="4">
         <v>194</v>
       </c>
       <c r="F26">
@@ -1395,123 +1368,123 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" s="6">
+      <c r="A27" s="5">
         <v>6</v>
       </c>
       <c r="B27">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C27">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D27">
-        <v>201</v>
-      </c>
-      <c r="E27" s="5">
+        <v>182</v>
+      </c>
+      <c r="E27" s="4">
         <v>192</v>
       </c>
       <c r="F27">
         <v>191</v>
       </c>
       <c r="G27">
-        <v>200</v>
+        <v>194</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A28" s="6">
+      <c r="A28" s="5">
         <v>7</v>
       </c>
       <c r="B28">
         <v>38</v>
       </c>
       <c r="C28">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D28">
-        <v>201</v>
-      </c>
-      <c r="E28" s="5">
+        <v>87</v>
+      </c>
+      <c r="E28" s="4">
         <v>190</v>
       </c>
       <c r="F28">
         <v>190</v>
       </c>
       <c r="G28">
-        <v>200</v>
+        <v>192</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A29" s="6">
+      <c r="A29" s="5">
         <v>8</v>
       </c>
       <c r="B29">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C29">
         <v>16</v>
       </c>
       <c r="D29">
-        <v>200</v>
-      </c>
-      <c r="E29" s="5">
+        <v>42</v>
+      </c>
+      <c r="E29" s="4">
         <v>188</v>
       </c>
       <c r="F29">
         <v>188</v>
       </c>
       <c r="G29">
-        <v>201</v>
+        <v>190</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="9" t="s">
+      <c r="A31" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B31" s="7"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="7"/>
+    </row>
+    <row r="32" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B32" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B31" s="9"/>
-      <c r="C31" s="9"/>
-      <c r="D31" s="9"/>
-      <c r="E31" s="9"/>
-      <c r="F31" s="9"/>
-      <c r="G31" s="9"/>
-    </row>
-    <row r="32" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B32" s="9" t="s">
+      <c r="C32" s="7"/>
+      <c r="D32" s="8"/>
+      <c r="E32" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C32" s="9"/>
-      <c r="D32" s="10"/>
-      <c r="E32" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="F32" s="9"/>
-      <c r="G32" s="9"/>
-    </row>
-    <row r="33" spans="1:7" s="3" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="8"/>
-      <c r="B33" s="2" t="s">
+      <c r="F32" s="7"/>
+      <c r="G32" s="7"/>
+    </row>
+    <row r="33" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="11"/>
+      <c r="B33" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="C33" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D33" s="2" t="s">
+      <c r="D33" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E33" s="4" t="s">
+      <c r="E33" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F33" s="2" t="s">
+      <c r="F33" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G33" s="2" t="s">
+      <c r="G33" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A34" s="1">
+      <c r="A34" s="5">
         <v>3</v>
       </c>
       <c r="B34">
@@ -1523,7 +1496,7 @@
       <c r="D34">
         <v>201</v>
       </c>
-      <c r="E34" s="5">
+      <c r="E34" s="4">
         <v>201</v>
       </c>
       <c r="F34">
@@ -1534,19 +1507,19 @@
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A35" s="1">
+      <c r="A35" s="5">
         <v>4</v>
       </c>
       <c r="B35">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C35">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="D35">
-        <v>200</v>
-      </c>
-      <c r="E35" s="5">
+        <v>201</v>
+      </c>
+      <c r="E35" s="4">
         <v>200</v>
       </c>
       <c r="F35">
@@ -1557,115 +1530,115 @@
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A36" s="1">
+      <c r="A36" s="5">
         <v>5</v>
       </c>
       <c r="B36">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C36">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="D36">
-        <v>200</v>
-      </c>
-      <c r="E36" s="5">
-        <v>194</v>
+        <v>197</v>
+      </c>
+      <c r="E36" s="4">
+        <v>198</v>
       </c>
       <c r="F36">
         <v>196</v>
       </c>
       <c r="G36">
-        <v>197</v>
+        <v>200</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A37" s="1">
+      <c r="A37" s="5">
         <v>6</v>
       </c>
       <c r="B37">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C37">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="D37">
-        <v>201</v>
-      </c>
-      <c r="E37" s="5">
+        <v>182</v>
+      </c>
+      <c r="E37" s="4">
         <v>192</v>
       </c>
       <c r="F37">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="G37">
-        <v>201</v>
+        <v>196</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A38" s="1">
+      <c r="A38" s="5">
         <v>7</v>
       </c>
       <c r="B38">
         <v>40</v>
       </c>
       <c r="C38">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D38">
-        <v>201</v>
-      </c>
-      <c r="E38" s="5">
+        <v>87</v>
+      </c>
+      <c r="E38" s="4">
         <v>190</v>
       </c>
       <c r="F38">
         <v>190</v>
       </c>
       <c r="G38">
-        <v>201</v>
+        <v>192</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A39" s="1">
+      <c r="A39" s="5">
         <v>8</v>
       </c>
       <c r="B39">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C39">
         <v>16</v>
       </c>
       <c r="D39">
-        <v>200</v>
-      </c>
-      <c r="E39" s="5">
+        <v>43</v>
+      </c>
+      <c r="E39" s="4">
         <v>188</v>
       </c>
       <c r="F39">
         <v>188</v>
       </c>
       <c r="G39">
-        <v>201</v>
+        <v>190</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A31:G31"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="E32:G32"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="E22:G22"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A11:G11"/>
     <mergeCell ref="A21:G21"/>
-    <mergeCell ref="A31:G31"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="E2:G2"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="E12:G12"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="E22:G22"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="E32:G32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>